<commit_message>
Update Master DB pages
</commit_message>
<xml_diff>
--- a/database/ipcdb rev02.xlsx
+++ b/database/ipcdb rev02.xlsx
@@ -1821,7 +1821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1891,11 +1891,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1903,20 +1903,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2209,8 +2212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
@@ -2310,42 +2313,42 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="27" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="28" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="28" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2356,7 +2359,7 @@
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" s="14" t="s">
         <v>115</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" s="15" t="s">
         <v>75</v>
       </c>
@@ -2378,7 +2381,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" s="15" t="s">
         <v>2</v>
       </c>
@@ -2389,7 +2392,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" s="15" t="s">
         <v>10</v>
       </c>
@@ -2400,7 +2403,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" s="15" t="s">
         <v>72</v>
       </c>
@@ -2411,7 +2414,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" s="15" t="s">
         <v>73</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" s="15" t="s">
         <v>37</v>
       </c>
@@ -2433,7 +2436,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" s="15" t="s">
         <v>35</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" s="15" t="s">
         <v>46</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" s="15" t="s">
         <v>6</v>
       </c>
@@ -2466,7 +2469,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="50.4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" ht="50.4" x14ac:dyDescent="0.5">
       <c r="A27" s="15" t="s">
         <v>39</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="50.4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" ht="50.4" x14ac:dyDescent="0.5">
       <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
@@ -2487,8 +2490,11 @@
       <c r="C28" s="15" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E28" s="13">
+        <v>869161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" s="15" t="s">
         <v>9</v>
       </c>
@@ -2498,8 +2504,12 @@
       <c r="C29" s="15" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E29" s="36">
+        <f>E28*7/107</f>
+        <v>56861</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" s="15" t="s">
         <v>44</v>
       </c>
@@ -2509,8 +2519,12 @@
       <c r="C30" s="15" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="E30" s="36">
+        <f>E28-E29</f>
+        <v>812300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" s="15" t="s">
         <v>45</v>
       </c>
@@ -2521,7 +2535,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" s="15" t="s">
         <v>29</v>
       </c>
@@ -3994,65 +4008,71 @@
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A139" s="31" t="s">
+      <c r="A139" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B139" s="28"/>
-      <c r="C139" s="28"/>
+      <c r="B139" s="34"/>
+      <c r="C139" s="34"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A140" s="28"/>
-      <c r="B140" s="28"/>
-      <c r="C140" s="28"/>
+      <c r="A140" s="34"/>
+      <c r="B140" s="34"/>
+      <c r="C140" s="34"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A141" s="28"/>
-      <c r="B141" s="28"/>
-      <c r="C141" s="28"/>
+      <c r="A141" s="34"/>
+      <c r="B141" s="34"/>
+      <c r="C141" s="34"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A142" s="28"/>
-      <c r="B142" s="28"/>
-      <c r="C142" s="28"/>
+      <c r="A142" s="34"/>
+      <c r="B142" s="34"/>
+      <c r="C142" s="34"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A143" s="28"/>
-      <c r="B143" s="28"/>
-      <c r="C143" s="28"/>
+      <c r="A143" s="34"/>
+      <c r="B143" s="34"/>
+      <c r="C143" s="34"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A144" s="26"/>
       <c r="B144" s="26"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A145" s="27" t="s">
+      <c r="A145" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="B145" s="28"/>
-      <c r="C145" s="28"/>
+      <c r="B145" s="34"/>
+      <c r="C145" s="34"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A146" s="28"/>
-      <c r="B146" s="28"/>
-      <c r="C146" s="28"/>
+      <c r="A146" s="34"/>
+      <c r="B146" s="34"/>
+      <c r="C146" s="34"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A147" s="28"/>
-      <c r="B147" s="28"/>
-      <c r="C147" s="28"/>
+      <c r="A147" s="34"/>
+      <c r="B147" s="34"/>
+      <c r="C147" s="34"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A148" s="28"/>
-      <c r="B148" s="28"/>
-      <c r="C148" s="28"/>
+      <c r="A148" s="34"/>
+      <c r="B148" s="34"/>
+      <c r="C148" s="34"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A149" s="28"/>
-      <c r="B149" s="28"/>
-      <c r="C149" s="28"/>
+      <c r="A149" s="34"/>
+      <c r="B149" s="34"/>
+      <c r="C149" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A145:C149"/>
+    <mergeCell ref="A116:C116"/>
+    <mergeCell ref="A121:C121"/>
+    <mergeCell ref="A128:C128"/>
+    <mergeCell ref="A111:C111"/>
+    <mergeCell ref="A139:C143"/>
     <mergeCell ref="A102:C102"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A6:C6"/>
@@ -4065,12 +4085,6 @@
     <mergeCell ref="A84:C84"/>
     <mergeCell ref="A92:C92"/>
     <mergeCell ref="A97:C97"/>
-    <mergeCell ref="A145:C149"/>
-    <mergeCell ref="A116:C116"/>
-    <mergeCell ref="A121:C121"/>
-    <mergeCell ref="A128:C128"/>
-    <mergeCell ref="A111:C111"/>
-    <mergeCell ref="A139:C143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add All Status Pages
</commit_message>
<xml_diff>
--- a/database/ipcdb rev02.xlsx
+++ b/database/ipcdb rev02.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="480">
   <si>
     <t>supplier_name</t>
   </si>
@@ -1648,7 +1648,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1695,65 +1695,45 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="TH Sarabun New"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="TH Sarabun New"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <strike/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="TH Sarabun New"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
       <strike/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="TH Sarabun New"/>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1781,6 +1761,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEDE7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1821,7 +1819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1848,6 +1846,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1859,66 +1863,69 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="22" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2212,1867 +2219,1899 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="12"/>
-    <col min="5" max="5" width="16.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.21875" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="12"/>
+    <col min="1" max="1" width="32.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="14"/>
+    <col min="5" max="5" width="16.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="15" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A2" s="14" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A7" s="14" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11" s="31" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" s="27" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="19" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A17" s="14" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="17" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="17" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="17" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A22" s="15" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="17" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="17" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A25" s="15" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="17" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="50.4" x14ac:dyDescent="0.5">
-      <c r="A27" s="15" t="s">
+    <row r="27" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="17" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="50.4" x14ac:dyDescent="0.5">
-      <c r="A28" s="15" t="s">
+    <row r="28" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="15">
         <v>869161</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="20">
         <f>E28*7/107</f>
         <v>56861</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A30" s="15" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="20">
         <f>E28-E29</f>
         <v>812300</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A31" s="15" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="17" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A32" s="15" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A33" s="15" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A35" s="29" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A36" s="14" t="s">
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="21" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A37" s="15" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="22">
         <v>0</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="22" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="22">
         <v>1</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="22" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="E39" s="17">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="22">
         <v>2</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="22" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="E40" s="17">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="22">
         <v>3</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="22" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A41" s="29" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A42" s="14" t="s">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="21" t="s">
         <v>342</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="21" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A43" s="15" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="17" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="22">
         <v>0</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="22" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A44" s="15" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="17" t="s">
         <v>468</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="22">
         <v>1</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="22" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="E45" s="17">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E45" s="22">
         <v>2</v>
       </c>
-      <c r="F45" s="17" t="s">
+      <c r="F45" s="22" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A46" s="29" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A47" s="14" t="s">
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A48" s="15" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="17" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A49" s="15" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A50" s="15" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A51" s="15" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A52" s="15" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A53" s="15" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="17" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A54" s="15" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="17" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A55" s="15" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A56" s="15" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A57" s="15" t="s">
+    <row r="57" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A59" s="29" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A60" s="14" t="s">
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A61" s="15" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="17" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A62" s="15" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A63" s="15" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="17" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A64" s="15" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="17" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A65" s="15" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="17" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A66" s="15" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C66" s="17" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A67" s="15" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C67" s="17" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A68" s="15" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C68" s="17" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A69" s="15" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="17" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A70" s="15" t="s">
+    <row r="70" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="17" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A71" s="15" t="s">
+    <row r="71" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="17" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A72" s="15" t="s">
+    <row r="72" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="C72" s="17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A73" s="15" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="C73" s="17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A74" s="15" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="C74" s="17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A75" s="15" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C75" s="15" t="s">
+      <c r="C75" s="17" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A76" s="15" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="C76" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A77" s="15" t="s">
+    <row r="77" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="C77" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A78" s="15" t="s">
+    <row r="78" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A78" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="C78" s="15" t="s">
+      <c r="C78" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A79" s="15" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B79" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C79" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A80" s="15" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="C80" s="17" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A81" s="15" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C81" s="17" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A82" s="15" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="17" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A84" s="29" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A85" s="14" t="s">
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A86" s="15" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A87" s="15" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C87" s="15" t="s">
+      <c r="C87" s="17" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A88" s="15" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="C88" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A89" s="15" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C89" s="15" t="s">
+      <c r="C89" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A90" s="15" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B90" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C90" s="15" t="s">
+      <c r="C90" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A91" s="18"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A92" s="29" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="23"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="B92" s="30"/>
-      <c r="C92" s="30"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A93" s="14" t="s">
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" s="16" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A94" s="15" t="s">
+      <c r="E93" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="F93" s="22" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="B94" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A95" s="15" t="s">
+      <c r="E94" s="22">
+        <v>1</v>
+      </c>
+      <c r="F94" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C95" s="15" t="s">
+      <c r="C95" s="17" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A97" s="29" t="s">
+      <c r="E95" s="22">
+        <v>2</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E96" s="22">
+        <v>3</v>
+      </c>
+      <c r="F96" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="B97" s="30"/>
-      <c r="C97" s="30"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A98" s="14" t="s">
+      <c r="B97" s="35"/>
+      <c r="C97" s="35"/>
+      <c r="E97" s="22">
+        <v>4</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C98" s="14" t="s">
+      <c r="C98" s="16" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A99" s="15" t="s">
+      <c r="E98" s="22">
+        <v>5</v>
+      </c>
+      <c r="F98" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C99" s="15" t="s">
+      <c r="C99" s="17" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A100" s="15" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C100" s="15" t="s">
+      <c r="C100" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A102" s="29" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B102" s="30"/>
-      <c r="C102" s="30"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A103" s="14" t="s">
+      <c r="B102" s="39"/>
+      <c r="C102" s="39"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C103" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E103" s="17" t="s">
+      <c r="E103" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F103" s="17" t="s">
+      <c r="F103" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="G103" s="17" t="s">
+      <c r="G103" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H103" s="17" t="s">
+      <c r="H103" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="I103" s="17" t="s">
+      <c r="I103" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="J103" s="17" t="s">
+      <c r="J103" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A104" s="15" t="s">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C104" s="15" t="s">
+      <c r="C104" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="E104" s="17">
+      <c r="E104" s="22">
         <v>1001</v>
       </c>
-      <c r="F104" s="17" t="s">
+      <c r="F104" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G104" s="17" t="s">
+      <c r="G104" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H104" s="17" t="s">
+      <c r="H104" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="I104" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J104" s="17"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A105" s="15" t="s">
+      <c r="I104" s="22">
+        <v>1</v>
+      </c>
+      <c r="J104" s="22"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C105" s="15" t="s">
+      <c r="C105" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E105" s="17">
+      <c r="E105" s="22">
         <v>1002</v>
       </c>
-      <c r="F105" s="17" t="s">
+      <c r="F105" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="G105" s="17" t="s">
+      <c r="G105" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H105" s="17" t="s">
+      <c r="H105" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="I105" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="J105" s="17"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A106" s="15" t="s">
+      <c r="I105" s="17">
+        <v>2</v>
+      </c>
+      <c r="J105" s="22"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B106" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C106" s="15" t="s">
+      <c r="C106" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="E106" s="17">
+      <c r="E106" s="22">
         <v>1003</v>
       </c>
-      <c r="F106" s="17" t="s">
+      <c r="F106" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="G106" s="17" t="s">
+      <c r="G106" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H106" s="17" t="s">
+      <c r="H106" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="I106" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J106" s="17"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A107" s="15" t="s">
+      <c r="I106" s="17">
+        <v>3</v>
+      </c>
+      <c r="J106" s="22"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C107" s="15" t="s">
+      <c r="C107" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E107" s="17">
+      <c r="E107" s="22">
         <v>1004</v>
       </c>
-      <c r="F107" s="17" t="s">
+      <c r="F107" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="G107" s="17" t="s">
+      <c r="G107" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H107" s="17" t="s">
+      <c r="H107" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="I107" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="J107" s="17"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A108" s="15" t="s">
+      <c r="I107" s="17">
+        <v>4</v>
+      </c>
+      <c r="J107" s="22"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B108" s="15" t="s">
+      <c r="B108" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C108" s="15" t="s">
+      <c r="C108" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="E108" s="17">
+      <c r="E108" s="22">
         <v>1005</v>
       </c>
-      <c r="F108" s="17" t="s">
+      <c r="F108" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="G108" s="17" t="s">
+      <c r="G108" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H108" s="17" t="s">
+      <c r="H108" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I108" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="J108" s="17"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A109" s="15" t="s">
+      <c r="I108" s="22">
+        <v>5</v>
+      </c>
+      <c r="J108" s="22"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C109" s="15" t="s">
+      <c r="C109" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A111" s="29" t="s">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="34" t="s">
         <v>353</v>
       </c>
-      <c r="B111" s="30"/>
-      <c r="C111" s="30"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A112" s="14" t="s">
+      <c r="B111" s="35"/>
+      <c r="C111" s="35"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="B112" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C112" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E112" s="16" t="s">
+      <c r="E112" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="F112" s="16" t="s">
+      <c r="F112" s="21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A113" s="15" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C113" s="15" t="s">
+      <c r="C113" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="E113" s="17">
+      <c r="E113" s="22">
         <v>0</v>
       </c>
-      <c r="F113" s="17" t="s">
+      <c r="F113" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A114" s="15" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B114" s="15" t="s">
+      <c r="B114" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C114" s="15" t="s">
+      <c r="C114" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="E114" s="17">
+      <c r="E114" s="22">
         <v>1</v>
       </c>
-      <c r="F114" s="17" t="s">
+      <c r="F114" s="22" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="E115" s="17">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E115" s="22">
         <v>2</v>
       </c>
-      <c r="F115" s="17" t="s">
+      <c r="F115" s="22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A116" s="29" t="s">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="34" t="s">
         <v>478</v>
       </c>
-      <c r="B116" s="30"/>
-      <c r="C116" s="30"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A117" s="14" t="s">
+      <c r="B116" s="35"/>
+      <c r="C116" s="35"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="B117" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C117" s="14" t="s">
+      <c r="C117" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E117" s="16" t="s">
+      <c r="E117" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F117" s="16" t="s">
+      <c r="F117" s="21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A118" s="15" t="s">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C118" s="15" t="s">
+      <c r="C118" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E118" s="17">
+      <c r="E118" s="22">
         <v>1</v>
       </c>
-      <c r="F118" s="17" t="s">
+      <c r="F118" s="22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A119" s="15" t="s">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C119" s="15" t="s">
+      <c r="C119" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E119" s="17">
+      <c r="E119" s="22">
         <v>2</v>
       </c>
-      <c r="F119" s="17" t="s">
+      <c r="F119" s="22" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A121" s="29" t="s">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="B121" s="30"/>
-      <c r="C121" s="30"/>
-    </row>
-    <row r="122" spans="1:8" ht="27.6" x14ac:dyDescent="0.5">
-      <c r="A122" s="14" t="s">
+      <c r="B121" s="39"/>
+      <c r="C121" s="39"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="B122" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C122" s="14" t="s">
+      <c r="C122" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E122" s="19" t="s">
+      <c r="E122" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="F122" s="16" t="s">
+      <c r="F122" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G122" s="19" t="s">
+      <c r="G122" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H122" s="19" t="s">
+      <c r="H122" s="17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A123" s="15" t="s">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="B123" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C123" s="15" t="s">
+      <c r="C123" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="E123" s="19">
+      <c r="E123" s="17">
         <v>1</v>
       </c>
-      <c r="F123" s="17">
+      <c r="F123" s="22">
         <v>1</v>
       </c>
-      <c r="G123" s="19">
+      <c r="G123" s="17">
         <v>1</v>
       </c>
-      <c r="H123" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A124" s="15" t="s">
+      <c r="H123" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B124" s="15" t="s">
+      <c r="B124" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C124" s="15" t="s">
+      <c r="C124" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E124" s="19">
+      <c r="E124" s="17">
         <v>2</v>
       </c>
-      <c r="F124" s="17">
+      <c r="F124" s="22">
         <v>1</v>
       </c>
-      <c r="G124" s="19">
+      <c r="G124" s="17">
         <v>2</v>
       </c>
-      <c r="H124" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A125" s="15" t="s">
+      <c r="H124" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B125" s="15" t="s">
+      <c r="B125" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C125" s="15" t="s">
+      <c r="C125" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E125" s="17">
+      <c r="E125" s="22">
         <v>3</v>
       </c>
-      <c r="F125" s="17">
+      <c r="F125" s="22">
         <v>1</v>
       </c>
-      <c r="G125" s="17">
+      <c r="G125" s="22">
         <v>3</v>
       </c>
-      <c r="H125" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A126" s="15" t="s">
+      <c r="H125" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B126" s="15" t="s">
+      <c r="B126" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C126" s="15" t="s">
+      <c r="C126" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E126" s="17">
+      <c r="E126" s="22">
         <v>4</v>
       </c>
-      <c r="F126" s="17">
+      <c r="F126" s="22">
         <v>2</v>
       </c>
-      <c r="G126" s="17">
+      <c r="G126" s="22">
         <v>3</v>
       </c>
-      <c r="H126" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="E127" s="17">
+      <c r="H126" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E127" s="22">
         <v>5</v>
       </c>
-      <c r="F127" s="17">
+      <c r="F127" s="22">
         <v>2</v>
       </c>
-      <c r="G127" s="17">
+      <c r="G127" s="22">
         <v>4</v>
       </c>
-      <c r="H127" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A128" s="29" t="s">
+      <c r="H127" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="B128" s="30"/>
-      <c r="C128" s="30"/>
-    </row>
-    <row r="129" spans="1:12" ht="27.6" x14ac:dyDescent="0.5">
-      <c r="A129" s="14" t="s">
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B129" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C129" s="14" t="s">
+      <c r="C129" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E129" s="19" t="s">
+      <c r="E129" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="F129" s="19" t="s">
+      <c r="F129" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G129" s="19" t="s">
+      <c r="G129" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H129" s="19" t="s">
+      <c r="H129" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I129" s="19" t="s">
+      <c r="I129" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="J129" s="19" t="s">
+      <c r="J129" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K129" s="19" t="s">
+      <c r="K129" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L129" s="19" t="s">
+      <c r="L129" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A130" s="15" t="s">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B130" s="15" t="s">
+      <c r="B130" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C130" s="15" t="s">
+      <c r="C130" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E130" s="20">
+      <c r="E130" s="24">
         <v>1</v>
       </c>
-      <c r="F130" s="20">
+      <c r="F130" s="24">
         <v>1</v>
       </c>
-      <c r="G130" s="20">
+      <c r="G130" s="24">
         <v>1</v>
       </c>
-      <c r="H130" s="20">
+      <c r="H130" s="24">
         <v>1</v>
       </c>
-      <c r="I130" s="20">
+      <c r="I130" s="24">
         <v>1002</v>
       </c>
-      <c r="J130" s="20" t="s">
+      <c r="J130" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="K130" s="20" t="s">
+      <c r="K130" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="L130" s="20" t="s">
+      <c r="L130" s="24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A131" s="15" t="s">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B131" s="15" t="s">
+      <c r="B131" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C131" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="E131" s="20">
+      <c r="E131" s="24">
         <v>2</v>
       </c>
-      <c r="F131" s="20">
+      <c r="F131" s="24">
         <v>1</v>
       </c>
-      <c r="G131" s="20">
+      <c r="G131" s="24">
         <v>1</v>
       </c>
-      <c r="H131" s="20">
+      <c r="H131" s="24">
         <v>2</v>
       </c>
-      <c r="I131" s="20">
+      <c r="I131" s="24">
         <v>1003</v>
       </c>
-      <c r="J131" s="20" t="s">
+      <c r="J131" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="K131" s="20" t="s">
+      <c r="K131" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="L131" s="20" t="s">
+      <c r="L131" s="24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A132" s="15" t="s">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B132" s="15" t="s">
+      <c r="B132" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C132" s="15" t="s">
+      <c r="C132" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="E132" s="20">
+      <c r="E132" s="24">
         <v>3</v>
       </c>
-      <c r="F132" s="20">
+      <c r="F132" s="24">
         <v>1</v>
       </c>
-      <c r="G132" s="20">
+      <c r="G132" s="24">
         <v>1</v>
       </c>
-      <c r="H132" s="20">
+      <c r="H132" s="24">
         <v>3</v>
       </c>
-      <c r="I132" s="20">
+      <c r="I132" s="24">
         <v>1004</v>
       </c>
-      <c r="J132" s="20" t="s">
+      <c r="J132" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="K132" s="20" t="s">
+      <c r="K132" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="L132" s="20" t="s">
+      <c r="L132" s="24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A133" s="15" t="s">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B133" s="15" t="s">
+      <c r="B133" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C133" s="15" t="s">
+      <c r="C133" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E133" s="21">
+      <c r="E133" s="25">
         <v>4</v>
       </c>
-      <c r="F133" s="21">
+      <c r="F133" s="25">
         <v>1</v>
       </c>
-      <c r="G133" s="21">
+      <c r="G133" s="25">
         <v>2</v>
       </c>
-      <c r="H133" s="21">
+      <c r="H133" s="25">
         <v>1</v>
       </c>
-      <c r="I133" s="21">
+      <c r="I133" s="25">
         <v>1002</v>
       </c>
-      <c r="J133" s="21" t="s">
+      <c r="J133" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="K133" s="22">
+      <c r="K133" s="26">
         <v>45500.625</v>
       </c>
-      <c r="L133" s="21" t="s">
+      <c r="L133" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A134" s="15" t="s">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B134" s="15" t="s">
+      <c r="B134" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C134" s="15" t="s">
+      <c r="C134" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E134" s="21">
+      <c r="E134" s="25">
         <v>5</v>
       </c>
-      <c r="F134" s="21">
+      <c r="F134" s="25">
         <v>1</v>
       </c>
-      <c r="G134" s="21">
+      <c r="G134" s="25">
         <v>2</v>
       </c>
-      <c r="H134" s="21">
+      <c r="H134" s="25">
         <v>2</v>
       </c>
-      <c r="I134" s="21">
+      <c r="I134" s="25">
         <v>1003</v>
       </c>
-      <c r="J134" s="21" t="s">
+      <c r="J134" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="K134" s="22">
+      <c r="K134" s="26">
         <v>45500.645833333336</v>
       </c>
-      <c r="L134" s="21" t="s">
+      <c r="L134" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A135" s="15" t="s">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B135" s="15" t="s">
+      <c r="B135" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C135" s="15" t="s">
+      <c r="C135" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E135" s="21">
+      <c r="E135" s="25">
         <v>6</v>
       </c>
-      <c r="F135" s="21">
+      <c r="F135" s="25">
         <v>1</v>
       </c>
-      <c r="G135" s="21">
+      <c r="G135" s="25">
         <v>2</v>
       </c>
-      <c r="H135" s="21">
+      <c r="H135" s="25">
         <v>3</v>
       </c>
-      <c r="I135" s="21">
+      <c r="I135" s="25">
         <v>1004</v>
       </c>
-      <c r="J135" s="21" t="s">
+      <c r="J135" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="K135" s="21" t="s">
+      <c r="K135" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="L135" s="21" t="s">
+      <c r="L135" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A136" s="15" t="s">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B136" s="15" t="s">
+      <c r="B136" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C136" s="15" t="s">
+      <c r="C136" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E136" s="23">
+      <c r="E136" s="27">
         <v>7</v>
       </c>
-      <c r="F136" s="23">
+      <c r="F136" s="27">
         <v>2</v>
       </c>
-      <c r="G136" s="23">
+      <c r="G136" s="27">
         <v>1</v>
       </c>
-      <c r="H136" s="24">
+      <c r="H136" s="28">
         <v>4</v>
       </c>
-      <c r="I136" s="24">
+      <c r="I136" s="28">
         <v>1004</v>
       </c>
-      <c r="J136" s="23" t="s">
+      <c r="J136" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="K136" s="25">
+      <c r="K136" s="29">
         <v>45500.625</v>
       </c>
-      <c r="L136" s="23" t="s">
+      <c r="L136" s="27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A137" s="15" t="s">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B137" s="15" t="s">
+      <c r="B137" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C137" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="E137" s="23">
+      <c r="E137" s="27">
         <v>8</v>
       </c>
-      <c r="F137" s="23">
+      <c r="F137" s="27">
         <v>2</v>
       </c>
-      <c r="G137" s="23">
+      <c r="G137" s="27">
         <v>1</v>
       </c>
-      <c r="H137" s="24">
+      <c r="H137" s="28">
         <v>5</v>
       </c>
-      <c r="I137" s="24">
+      <c r="I137" s="28">
         <v>1005</v>
       </c>
-      <c r="J137" s="23" t="s">
+      <c r="J137" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="K137" s="23" t="s">
+      <c r="K137" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="L137" s="23" t="s">
+      <c r="L137" s="27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A139" s="35" t="s">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B139" s="34"/>
-      <c r="C139" s="34"/>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A140" s="34"/>
-      <c r="B140" s="34"/>
-      <c r="C140" s="34"/>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A141" s="34"/>
-      <c r="B141" s="34"/>
-      <c r="C141" s="34"/>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A142" s="34"/>
-      <c r="B142" s="34"/>
-      <c r="C142" s="34"/>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A143" s="34"/>
-      <c r="B143" s="34"/>
-      <c r="C143" s="34"/>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A144" s="26"/>
-      <c r="B144" s="26"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B139" s="31"/>
+      <c r="C139" s="31"/>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" s="31"/>
+      <c r="B140" s="31"/>
+      <c r="C140" s="31"/>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141" s="31"/>
+      <c r="B141" s="31"/>
+      <c r="C141" s="31"/>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" s="31"/>
+      <c r="B142" s="31"/>
+      <c r="C142" s="31"/>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" s="31"/>
+      <c r="B143" s="31"/>
+      <c r="C143" s="31"/>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144" s="32"/>
+      <c r="B144" s="32"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="B145" s="34"/>
-      <c r="C145" s="34"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A146" s="34"/>
-      <c r="B146" s="34"/>
-      <c r="C146" s="34"/>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A147" s="34"/>
-      <c r="B147" s="34"/>
-      <c r="C147" s="34"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A148" s="34"/>
-      <c r="B148" s="34"/>
-      <c r="C148" s="34"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A149" s="34"/>
-      <c r="B149" s="34"/>
-      <c r="C149" s="34"/>
+      <c r="B145" s="31"/>
+      <c r="C145" s="31"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="31"/>
+      <c r="B146" s="31"/>
+      <c r="C146" s="31"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="31"/>
+      <c r="B147" s="31"/>
+      <c r="C147" s="31"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="31"/>
+      <c r="B148" s="31"/>
+      <c r="C148" s="31"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="31"/>
+      <c r="B149" s="31"/>
+      <c r="C149" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A145:C149"/>
-    <mergeCell ref="A116:C116"/>
-    <mergeCell ref="A121:C121"/>
-    <mergeCell ref="A128:C128"/>
-    <mergeCell ref="A111:C111"/>
-    <mergeCell ref="A139:C143"/>
     <mergeCell ref="A102:C102"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A6:C6"/>
@@ -4085,6 +4124,12 @@
     <mergeCell ref="A84:C84"/>
     <mergeCell ref="A92:C92"/>
     <mergeCell ref="A97:C97"/>
+    <mergeCell ref="A145:C149"/>
+    <mergeCell ref="A116:C116"/>
+    <mergeCell ref="A121:C121"/>
+    <mergeCell ref="A128:C128"/>
+    <mergeCell ref="A111:C111"/>
+    <mergeCell ref="A139:C143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
revise at 2025/05/14 17:42
</commit_message>
<xml_diff>
--- a/database/ipcdb rev02.xlsx
+++ b/database/ipcdb rev02.xlsx
@@ -1182,17 +1182,6 @@
     <t>ตาราง: inspect_approvals (บันทึกการอนุมัติการตรวจสอบในแต่ละระดับ)</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: Json
-{
-"name" : "kongruksiam",
-"languages" : ["ไทย","จีน","ญี่ปุ่น"], 
-"general" : {
-"weight":70,
-"height":175,
-}
-</t>
-  </si>
-  <si>
     <t>ขอคำสั่งในการสร้างตารางบน mySQL โดยมีข้อมูลตามนี้</t>
   </si>
   <si>
@@ -1545,9 +1534,6 @@
   </si>
   <si>
     <t>สถานะปัจจุบันของ Workflow (เช่น รอดำเนินการ, อนุมัติ, ไม่อนุมัติ) = approval_status</t>
-  </si>
-  <si>
-    <t>ตาราง: po_period</t>
   </si>
   <si>
     <t>รหัสงวด PO(Primary Key, Auto Increment)</t>
@@ -1737,9 +1723,6 @@
     <t>รหัสผู้ใช้ของผู้รับผิดชอบการอนุมัติในระดับนี้ หรืออาจะเปลี่ยนเป็น role การอนุมัติแทนก็ได้</t>
   </si>
   <si>
-    <t>ตาราง: inspection_approvals (ติดตามสถานะการอนุมัติของแต่ละ period ในแต่ละระดับการอนุมัติ)</t>
-  </si>
-  <si>
     <t>inspection_approval_id</t>
   </si>
   <si>
@@ -1846,6 +1829,23 @@
   </si>
   <si>
     <t>IPC ทั่วไป</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Json
+{
+"name" : "nathapat",
+"languages" : ["ไทย","จีน","ญี่ปุ่น"], 
+"general" : {
+"weight":65,
+"height":166,
+}
+</t>
+  </si>
+  <si>
+    <t>ตาราง: inspection_period_approvals (ติดตามสถานะการอนุมัติของแต่ละ period ในแต่ละระดับการอนุมัติ)</t>
+  </si>
+  <si>
+    <t>ตาราง: po_periods</t>
   </si>
 </sst>
 </file>
@@ -2146,7 +2146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2292,16 +2292,7 @@
     <xf numFmtId="0" fontId="13" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2310,19 +2301,22 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2337,8 +2331,17 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2629,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N186"/>
+  <dimension ref="A1:N189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2653,11 +2656,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -2693,11 +2696,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
     </row>
@@ -2745,11 +2748,11 @@
       <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -2790,16 +2793,16 @@
       <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="56" t="s">
+        <v>480</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="E16" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>482</v>
-      </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="E16" s="16" t="s">
-        <v>483</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2816,12 +2819,12 @@
         <v>0</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>115</v>
@@ -2833,12 +2836,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>116</v>
@@ -2850,7 +2853,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2858,7 +2861,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2866,15 +2869,15 @@
       <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="56" t="s">
         <v>322</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
       <c r="E23" s="16" t="s">
         <v>314</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -2913,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2924,13 +2927,13 @@
         <v>116</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E26" s="17">
         <v>2</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -2940,11 +2943,11 @@
       <c r="N27" s="10"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="s">
-        <v>451</v>
-      </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
+      <c r="A28" s="60" t="s">
+        <v>449</v>
+      </c>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -2967,14 +2970,14 @@
         <v>115</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>119</v>
@@ -3072,7 +3075,7 @@
         <v>126</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
@@ -3083,7 +3086,7 @@
         <v>126</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E40" s="10">
         <v>869161</v>
@@ -3249,21 +3252,21 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B52" s="32" t="s">
         <v>116</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
@@ -3274,22 +3277,22 @@
         <v>121</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A54" s="64" t="s">
-        <v>479</v>
-      </c>
-      <c r="B54" s="65"/>
-      <c r="C54" s="65"/>
+      <c r="A54" s="62" t="s">
+        <v>477</v>
+      </c>
+      <c r="B54" s="63"/>
+      <c r="C54" s="63"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="59" t="s">
-        <v>448</v>
-      </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="60"/>
+      <c r="A56" s="60" t="s">
+        <v>530</v>
+      </c>
+      <c r="B56" s="61"/>
+      <c r="C56" s="61"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
@@ -3304,13 +3307,13 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B58" s="32" t="s">
         <v>115</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3321,12 +3324,12 @@
         <v>133</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B60" s="32" t="s">
         <v>133</v>
@@ -3337,13 +3340,13 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B61" s="45" t="s">
         <v>126</v>
       </c>
       <c r="C61" s="44" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3354,18 +3357,18 @@
         <v>116</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B63" s="32" t="s">
         <v>116</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3409,7 +3412,7 @@
         <v>126</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3431,7 +3434,7 @@
         <v>126</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3453,7 +3456,7 @@
         <v>126</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3552,7 +3555,7 @@
         <v>116</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3563,24 +3566,24 @@
         <v>133</v>
       </c>
       <c r="C81" s="42" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A82" s="66" t="s">
-        <v>480</v>
-      </c>
-      <c r="B82" s="67"/>
-      <c r="C82" s="67"/>
+      <c r="A82" s="64" t="s">
+        <v>478</v>
+      </c>
+      <c r="B82" s="65"/>
+      <c r="C82" s="65"/>
       <c r="E82" s="17"/>
       <c r="F82" s="17"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="59" t="s">
-        <v>471</v>
-      </c>
-      <c r="B84" s="60"/>
-      <c r="C84" s="60"/>
+      <c r="A84" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="B84" s="61"/>
+      <c r="C84" s="61"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
@@ -3595,7 +3598,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B86" s="32" t="s">
         <v>115</v>
@@ -3606,13 +3609,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B87" s="32" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3620,15 +3623,15 @@
         <v>74</v>
       </c>
       <c r="B88" s="45" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C88" s="44" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B89" s="32" t="s">
         <v>133</v>
@@ -3645,7 +3648,7 @@
         <v>126</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3656,7 +3659,7 @@
         <v>126</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3667,18 +3670,18 @@
         <v>126</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B93" s="32" t="s">
         <v>126</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3689,7 +3692,7 @@
         <v>126</v>
       </c>
       <c r="C94" s="51" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3700,7 +3703,7 @@
         <v>126</v>
       </c>
       <c r="C95" s="51" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3711,7 +3714,7 @@
         <v>126</v>
       </c>
       <c r="C96" s="51" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3837,50 +3840,50 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B108" s="32" t="s">
         <v>116</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B109" s="32" t="s">
         <v>133</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B110" s="32" t="s">
         <v>157</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A111" s="66" t="s">
-        <v>481</v>
-      </c>
-      <c r="B111" s="67"/>
-      <c r="C111" s="67"/>
+      <c r="A111" s="64" t="s">
+        <v>479</v>
+      </c>
+      <c r="B111" s="65"/>
+      <c r="C111" s="65"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="59" t="s">
-        <v>473</v>
-      </c>
-      <c r="B113" s="60"/>
-      <c r="C113" s="60"/>
+      <c r="A113" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="B113" s="61"/>
+      <c r="C113" s="61"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
@@ -3895,7 +3898,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B115" s="32" t="s">
         <v>115</v>
@@ -3906,13 +3909,13 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B116" s="32" t="s">
         <v>133</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3954,11 +3957,11 @@
       <c r="C120" s="18"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="57" t="s">
+      <c r="A121" s="54" t="s">
         <v>316</v>
       </c>
-      <c r="B121" s="58"/>
-      <c r="C121" s="58"/>
+      <c r="B121" s="55"/>
+      <c r="C121" s="55"/>
       <c r="E121" s="17" t="s">
         <v>317</v>
       </c>
@@ -4026,11 +4029,11 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="55" t="s">
+      <c r="A126" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="B126" s="56"/>
-      <c r="C126" s="56"/>
+      <c r="B126" s="57"/>
+      <c r="C126" s="57"/>
       <c r="E126" s="17">
         <v>5</v>
       </c>
@@ -4072,11 +4075,11 @@
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
+      <c r="A131" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="B131" s="58"/>
-      <c r="C131" s="58"/>
+      <c r="B131" s="55"/>
+      <c r="C131" s="55"/>
       <c r="E131" s="17" t="s">
         <v>89</v>
       </c>
@@ -4254,11 +4257,11 @@
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" s="55" t="s">
+      <c r="A140" s="56" t="s">
         <v>325</v>
       </c>
-      <c r="B140" s="56"/>
-      <c r="C140" s="56"/>
+      <c r="B140" s="57"/>
+      <c r="C140" s="57"/>
       <c r="E140" s="47" t="s">
         <v>107</v>
       </c>
@@ -4285,7 +4288,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B142" s="32" t="s">
         <v>115</v>
@@ -4302,13 +4305,13 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B143" s="32" t="s">
         <v>116</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E143" s="17">
         <v>2</v>
@@ -4318,16 +4321,16 @@
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A145" s="55" t="s">
-        <v>523</v>
-      </c>
-      <c r="B145" s="56"/>
-      <c r="C145" s="56"/>
+      <c r="A145" s="56" t="s">
+        <v>520</v>
+      </c>
+      <c r="B145" s="57"/>
+      <c r="C145" s="57"/>
       <c r="E145" s="47" t="s">
+        <v>518</v>
+      </c>
+      <c r="F145" s="16" t="s">
         <v>521</v>
-      </c>
-      <c r="F145" s="16" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -4344,45 +4347,45 @@
         <v>1</v>
       </c>
       <c r="F146" s="17" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B147" s="32" t="s">
         <v>115</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E147" s="17">
         <v>2</v>
       </c>
       <c r="F147" s="17" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B148" s="32" t="s">
         <v>116</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E148" s="17"/>
       <c r="F148" s="17"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A150" s="55" t="s">
-        <v>487</v>
-      </c>
-      <c r="B150" s="56"/>
-      <c r="C150" s="56"/>
+      <c r="A150" s="56" t="s">
+        <v>485</v>
+      </c>
+      <c r="B150" s="57"/>
+      <c r="C150" s="57"/>
       <c r="E150" s="46" t="s">
         <v>78</v>
       </c>
@@ -4390,7 +4393,7 @@
         <v>77</v>
       </c>
       <c r="G150" s="17" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -4407,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="F151" s="30" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="G151" s="17">
         <v>1</v>
@@ -4427,7 +4430,7 @@
         <v>2</v>
       </c>
       <c r="F152" s="17" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G152" s="17">
         <v>2</v>
@@ -4446,29 +4449,29 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B154" s="32" t="s">
         <v>121</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" s="57" t="s">
-        <v>510</v>
-      </c>
-      <c r="B156" s="58"/>
-      <c r="C156" s="58"/>
+      <c r="A156" s="54" t="s">
+        <v>507</v>
+      </c>
+      <c r="B156" s="55"/>
+      <c r="C156" s="55"/>
       <c r="E156" s="21" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F156" s="46" t="s">
         <v>78</v>
       </c>
       <c r="G156" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H156" s="12" t="s">
         <v>65</v>
@@ -4499,13 +4502,13 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B158" s="32" t="s">
         <v>115</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E158" s="26">
         <v>2</v>
@@ -4545,13 +4548,13 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B160" s="32" t="s">
         <v>133</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E160" s="17">
         <v>4</v>
@@ -4574,7 +4577,7 @@
         <v>116</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E161" s="17">
         <v>5</v>
@@ -4590,22 +4593,22 @@
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A163" s="59" t="s">
-        <v>494</v>
-      </c>
-      <c r="B163" s="60"/>
-      <c r="C163" s="60"/>
+      <c r="A163" s="60" t="s">
+        <v>529</v>
+      </c>
+      <c r="B163" s="61"/>
+      <c r="C163" s="61"/>
       <c r="E163" s="12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F163" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G163" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H163" s="21" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I163" s="12" t="s">
         <v>65</v>
@@ -4657,13 +4660,13 @@
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B165" s="32" t="s">
         <v>115</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E165" s="31">
         <v>2</v>
@@ -4692,13 +4695,13 @@
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B166" s="32" t="s">
         <v>121</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E166" s="31">
         <v>3</v>
@@ -4727,13 +4730,13 @@
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B167" s="32" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C167" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E167" s="19">
         <v>4</v>
@@ -4765,10 +4768,10 @@
         <v>74</v>
       </c>
       <c r="B168" s="45" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C168" s="44" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E168" s="19">
         <v>5</v>
@@ -4797,7 +4800,7 @@
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B169" s="32" t="s">
         <v>133</v>
@@ -4832,13 +4835,13 @@
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B170" s="32" t="s">
         <v>121</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E170" s="21">
         <v>7</v>
@@ -4902,97 +4905,119 @@
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B172" s="32" t="s">
         <v>121</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B173" s="32" t="s">
         <v>130</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B174" s="32" t="s">
         <v>116</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A176" s="61" t="s">
-        <v>489</v>
-      </c>
-      <c r="B176" s="54"/>
-      <c r="C176" s="54"/>
+      <c r="A176" s="68" t="s">
+        <v>487</v>
+      </c>
+      <c r="B176" s="67"/>
+      <c r="C176" s="67"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="54"/>
-      <c r="B177" s="54"/>
-      <c r="C177" s="54"/>
+      <c r="A177" s="67"/>
+      <c r="B177" s="67"/>
+      <c r="C177" s="67"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="54"/>
-      <c r="B178" s="54"/>
-      <c r="C178" s="54"/>
+      <c r="A178" s="67"/>
+      <c r="B178" s="67"/>
+      <c r="C178" s="67"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="54"/>
-      <c r="B179" s="54"/>
-      <c r="C179" s="54"/>
+      <c r="A179" s="67"/>
+      <c r="B179" s="67"/>
+      <c r="C179" s="67"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="54"/>
-      <c r="B180" s="54"/>
-      <c r="C180" s="54"/>
+      <c r="A180" s="67"/>
+      <c r="B180" s="67"/>
+      <c r="C180" s="67"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="24"/>
       <c r="B181" s="38"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="53" t="s">
-        <v>329</v>
-      </c>
-      <c r="B182" s="54"/>
-      <c r="C182" s="54"/>
+      <c r="A182" s="66" t="s">
+        <v>528</v>
+      </c>
+      <c r="B182" s="67"/>
+      <c r="C182" s="67"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="54"/>
-      <c r="B183" s="54"/>
-      <c r="C183" s="54"/>
+      <c r="A183" s="67"/>
+      <c r="B183" s="67"/>
+      <c r="C183" s="67"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="54"/>
-      <c r="B184" s="54"/>
-      <c r="C184" s="54"/>
+      <c r="A184" s="67"/>
+      <c r="B184" s="67"/>
+      <c r="C184" s="67"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="54"/>
-      <c r="B185" s="54"/>
-      <c r="C185" s="54"/>
+      <c r="A185" s="67"/>
+      <c r="B185" s="67"/>
+      <c r="C185" s="67"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="54"/>
-      <c r="B186" s="54"/>
-      <c r="C186" s="54"/>
+      <c r="A186" s="67"/>
+      <c r="B186" s="67"/>
+      <c r="C186" s="67"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="69"/>
+      <c r="B187" s="69"/>
+      <c r="C187" s="69"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="69"/>
+      <c r="B188" s="69"/>
+      <c r="C188" s="69"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="69"/>
+      <c r="B189" s="69"/>
+      <c r="C189" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A150:C150"/>
+    <mergeCell ref="A156:C156"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="A140:C140"/>
+    <mergeCell ref="A176:C180"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A182:C189"/>
     <mergeCell ref="A131:C131"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A6:C6"/>
@@ -5008,13 +5033,6 @@
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="A82:C82"/>
     <mergeCell ref="A111:C111"/>
-    <mergeCell ref="A182:C186"/>
-    <mergeCell ref="A150:C150"/>
-    <mergeCell ref="A156:C156"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="A140:C140"/>
-    <mergeCell ref="A176:C180"/>
-    <mergeCell ref="A145:C145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5896,7 +5914,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -5906,12 +5924,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -5921,7 +5939,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
@@ -5931,12 +5949,12 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -5946,7 +5964,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
@@ -5956,12 +5974,12 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -5971,7 +5989,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
@@ -5981,27 +5999,27 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
@@ -6016,62 +6034,62 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -6081,22 +6099,22 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
@@ -6106,22 +6124,22 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
@@ -6131,7 +6149,7 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
@@ -6141,12 +6159,12 @@
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
@@ -6166,37 +6184,37 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
@@ -6206,7 +6224,7 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
@@ -6216,12 +6234,12 @@
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
@@ -6231,92 +6249,92 @@
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
@@ -6326,12 +6344,12 @@
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
@@ -6341,7 +6359,7 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
@@ -6351,12 +6369,12 @@
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
@@ -6366,17 +6384,17 @@
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
@@ -6386,22 +6404,22 @@
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
@@ -6411,7 +6429,7 @@
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
@@ -6421,12 +6439,12 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
@@ -6436,7 +6454,7 @@
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
@@ -6446,17 +6464,17 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
@@ -6466,22 +6484,22 @@
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
@@ -6491,7 +6509,7 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
@@ -6501,12 +6519,12 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
@@ -6516,7 +6534,7 @@
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
@@ -6526,12 +6544,12 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
@@ -6541,7 +6559,7 @@
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
@@ -6551,12 +6569,12 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
@@ -6566,17 +6584,17 @@
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
@@ -6586,7 +6604,7 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
@@ -6596,12 +6614,12 @@
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
@@ -6611,47 +6629,47 @@
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
@@ -6679,7 +6697,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.3">
@@ -7349,7 +7367,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.3">

</xml_diff>